<commit_message>
fix POST API Server
</commit_message>
<xml_diff>
--- a/bill_test.xlsx
+++ b/bill_test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\Projects\Webs\Javascript\Projects\manage-housecharge-MERN-stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B1D80B7-0C25-4491-93C3-57FA97981F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B65ED6B-9E7C-4C3D-986E-3E38EE78E2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bill_test" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -905,14 +905,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1437,5 +1437,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>